<commit_message>
Bot already work and autodeployed with units tests
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_10\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C504E84-7CF1-4EAA-B27C-38086F8CE243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D05311-7EFA-4C83-A22E-EF6657A2AE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,8 +702,8 @@
       <c r="C4" s="19"/>
       <c r="D4" s="7"/>
       <c r="F4" s="3">
-        <f>AVERAGE(C5:C7,C9:C13,C15:C18,)</f>
-        <v>0</v>
+        <f>AVERAGE(C5:C7,C9:C13,C15:C18)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -711,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -720,7 +720,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -729,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -745,7 +745,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -754,7 +754,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6"/>
       <c r="G10" s="13"/>
@@ -764,7 +764,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -773,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -782,7 +782,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6"/>
     </row>
@@ -798,7 +798,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="6"/>
     </row>
@@ -807,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="6"/>
     </row>
@@ -816,7 +816,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="6"/>
     </row>
@@ -825,7 +825,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4"/>
     </row>

</xml_diff>